<commit_message>
Excel Export Workinggit add calc
</commit_message>
<xml_diff>
--- a/calc/main/templates/OutputTemplate.xlsx
+++ b/calc/main/templates/OutputTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarsuDIOS666\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarsuDIOS666\Desktop\calcV2\calc\main\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C1AC67-D20D-4E14-A8EE-F2FC50EE3456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F94128-2F5A-479B-8617-8A2462BBA036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimación" sheetId="2" r:id="rId1"/>
@@ -706,13 +706,13 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="92.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="152.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>